<commit_message>
Updated latest set of sripts
</commit_message>
<xml_diff>
--- a/Datasets/Variation-in-PIT-Counts-2007-2016.xlsx
+++ b/Datasets/Variation-in-PIT-Counts-2007-2016.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{51BDDC9C-3026-4828-BE93-FE0E3B3005D7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{51BDDC9C-3026-4828-BE93-FE0E3B3005D7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Variation-in-PIT-Counts" sheetId="1" r:id="rId1"/>
+    <sheet name="Variation-with-TrendLines" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Variation-in-PIT-Counts'!$A$1:$J$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'Variation-with-TrendLines'!$A$1:$J$55</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
   <si>
     <t>state</t>
   </si>
@@ -582,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7F653F-455C-4C86-8854-1B6D20336E15}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -2360,4 +2362,2022 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF89203B-0F6F-43F9-B7E6-D64AC1D80860}">
+  <dimension ref="A1:J55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-0.67075499999999999</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-0.670207</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-0.33480900000000002</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-0.28656799999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-0.29343999999999998</v>
+      </c>
+      <c r="G2" s="1">
+        <v>-0.26016499999999998</v>
+      </c>
+      <c r="H2" s="1">
+        <v>-0.19181100000000001</v>
+      </c>
+      <c r="I2" s="1">
+        <v>-0.23808000000000001</v>
+      </c>
+      <c r="J2" s="1">
+        <v>-0.11411200000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-0.48625400000000002</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-0.35692600000000002</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-0.32455000000000001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-0.35247899999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-0.37080000000000002</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-0.317083</v>
+      </c>
+      <c r="H3" s="1">
+        <v>-0.25887399999999999</v>
+      </c>
+      <c r="I3" s="1">
+        <v>-0.23785500000000001</v>
+      </c>
+      <c r="J3" s="1">
+        <v>-0.119133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-0.474383</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-0.479292</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-0.29371599999999998</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-0.36026000000000002</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-0.29781200000000002</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-0.18986600000000001</v>
+      </c>
+      <c r="H4" s="1">
+        <v>-0.19218299999999999</v>
+      </c>
+      <c r="I4" s="1">
+        <v>-0.16742000000000001</v>
+      </c>
+      <c r="J4" s="1">
+        <v>-6.6328999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-0.42424200000000001</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-0.312004</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-0.167966</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-0.38736700000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-0.37268200000000001</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-0.424481</v>
+      </c>
+      <c r="H5" s="1">
+        <v>-0.38080399999999998</v>
+      </c>
+      <c r="I5" s="1">
+        <v>-0.31097900000000001</v>
+      </c>
+      <c r="J5" s="1">
+        <v>-0.244142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-0.41887000000000002</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-0.42468299999999998</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-0.37101800000000001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>-0.34164699999999998</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-0.37357400000000002</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-0.32097999999999999</v>
+      </c>
+      <c r="H6" s="1">
+        <v>-0.219247</v>
+      </c>
+      <c r="I6" s="1">
+        <v>-0.188559</v>
+      </c>
+      <c r="J6" s="1">
+        <v>-2.3481999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-0.392349</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-0.32342700000000002</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-0.16960500000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-0.13214699999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-7.0115999999999998E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-8.6898000000000003E-2</v>
+      </c>
+      <c r="H7" s="1">
+        <v>-5.5978E-2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>-7.267E-3</v>
+      </c>
+      <c r="J7" s="1">
+        <v>-5.4670999999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="1">
+        <v>-0.389982</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-0.43355500000000002</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-0.27600799999999998</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-0.29979499999999998</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-0.35902299999999998</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-0.29545500000000002</v>
+      </c>
+      <c r="H8" s="1">
+        <v>-0.29253099999999999</v>
+      </c>
+      <c r="I8" s="1">
+        <v>-0.238839</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.18694E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-0.35792499999999999</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-0.24331800000000001</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-0.13639599999999999</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-0.108255</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-0.28066600000000003</v>
+      </c>
+      <c r="G9" s="1">
+        <v>-0.41552</v>
+      </c>
+      <c r="H9" s="1">
+        <v>-0.35388199999999997</v>
+      </c>
+      <c r="I9" s="1">
+        <v>-0.161104</v>
+      </c>
+      <c r="J9" s="1">
+        <v>-3.7891000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-0.35686400000000001</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-0.25988899999999998</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-0.29191099999999998</v>
+      </c>
+      <c r="E10" s="1">
+        <v>-0.30969200000000002</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-0.28902</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-0.25593500000000002</v>
+      </c>
+      <c r="H10" s="1">
+        <v>-0.17796699999999999</v>
+      </c>
+      <c r="I10" s="1">
+        <v>-0.107123</v>
+      </c>
+      <c r="J10" s="1">
+        <v>-0.104699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>-0.34268500000000002</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-0.323959</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-0.36596299999999998</v>
+      </c>
+      <c r="E11" s="1">
+        <v>-0.34921400000000002</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-0.38455299999999998</v>
+      </c>
+      <c r="G11" s="1">
+        <v>-0.370784</v>
+      </c>
+      <c r="H11" s="1">
+        <v>-0.23934900000000001</v>
+      </c>
+      <c r="I11" s="1">
+        <v>-0.21863099999999999</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-6.3886999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-0.337225</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-0.222694</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-0.34060200000000002</v>
+      </c>
+      <c r="E12" s="1">
+        <v>-0.29202800000000001</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-7.5875999999999999E-2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>-0.141125</v>
+      </c>
+      <c r="H12" s="1">
+        <v>-8.0950999999999995E-2</v>
+      </c>
+      <c r="I12" s="1">
+        <v>-7.5082999999999997E-2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>-1.9099000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-0.30185800000000002</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-0.33093400000000001</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-0.39640999999999998</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-0.41688199999999997</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-0.407995</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-0.39171699999999998</v>
+      </c>
+      <c r="H13" s="1">
+        <v>-0.29883799999999999</v>
+      </c>
+      <c r="I13" s="1">
+        <v>-0.192167</v>
+      </c>
+      <c r="J13" s="1">
+        <v>-6.5209000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-0.27302500000000002</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-0.27130100000000001</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-0.68058200000000002</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-0.68001900000000004</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-0.57012200000000002</v>
+      </c>
+      <c r="G14" s="1">
+        <v>-0.48610399999999998</v>
+      </c>
+      <c r="H14" s="1">
+        <v>-0.23574400000000001</v>
+      </c>
+      <c r="I14" s="1">
+        <v>-0.13286999999999999</v>
+      </c>
+      <c r="J14" s="1">
+        <v>-2.1318E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1">
+        <v>-0.25834800000000002</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-0.28460000000000002</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-0.30901200000000001</v>
+      </c>
+      <c r="E15" s="1">
+        <v>-0.31856299999999999</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-0.302064</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-0.37082500000000002</v>
+      </c>
+      <c r="H15" s="1">
+        <v>8.1607499999999999E-2</v>
+      </c>
+      <c r="I15" s="1">
+        <v>5.2054200000000002E-2</v>
+      </c>
+      <c r="J15" s="1">
+        <v>5.9981899999999998E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>-0.25163000000000002</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-0.21285000000000001</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-0.17538200000000001</v>
+      </c>
+      <c r="E16" s="1">
+        <v>-0.194859</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-0.172675</v>
+      </c>
+      <c r="G16" s="1">
+        <v>-0.18057100000000001</v>
+      </c>
+      <c r="H16" s="1">
+        <v>-0.136685</v>
+      </c>
+      <c r="I16" s="1">
+        <v>-0.11574</v>
+      </c>
+      <c r="J16" s="1">
+        <v>-0.120437</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1">
+        <v>-0.24942</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-0.24942</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-0.348777</v>
+      </c>
+      <c r="E17" s="1">
+        <v>-0.348777</v>
+      </c>
+      <c r="F17" s="1">
+        <v>-0.37156299999999998</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-0.30261900000000003</v>
+      </c>
+      <c r="H17" s="1">
+        <v>-0.19723299999999999</v>
+      </c>
+      <c r="I17" s="1">
+        <v>-0.17589199999999999</v>
+      </c>
+      <c r="J17" s="1">
+        <v>-0.13921600000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="1">
+        <v>-0.24741299999999999</v>
+      </c>
+      <c r="C18" s="1">
+        <v>-0.35902800000000001</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-0.23519599999999999</v>
+      </c>
+      <c r="E18" s="1">
+        <v>-0.32085000000000002</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-0.23275799999999999</v>
+      </c>
+      <c r="G18" s="1">
+        <v>-0.163634</v>
+      </c>
+      <c r="H18" s="1">
+        <v>-4.2250999999999997E-2</v>
+      </c>
+      <c r="I18" s="1">
+        <v>8.8293300000000005E-2</v>
+      </c>
+      <c r="J18" s="1">
+        <v>9.0729999999999999E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1">
+        <v>-0.24596499999999999</v>
+      </c>
+      <c r="C19" s="1">
+        <v>-0.23686699999999999</v>
+      </c>
+      <c r="D19" s="1">
+        <v>-0.323849</v>
+      </c>
+      <c r="E19" s="1">
+        <v>-0.320046</v>
+      </c>
+      <c r="F19" s="1">
+        <v>-0.26034499999999999</v>
+      </c>
+      <c r="G19" s="1">
+        <v>-0.210789</v>
+      </c>
+      <c r="H19" s="1">
+        <v>-0.123267</v>
+      </c>
+      <c r="I19" s="1">
+        <v>-9.8663000000000001E-2</v>
+      </c>
+      <c r="J19" s="1">
+        <v>3.5516399999999997E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1">
+        <v>-0.220051</v>
+      </c>
+      <c r="C20" s="1">
+        <v>-0.30890800000000002</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-0.25927899999999998</v>
+      </c>
+      <c r="E20" s="1">
+        <v>-0.289657</v>
+      </c>
+      <c r="F20" s="1">
+        <v>-0.22378799999999999</v>
+      </c>
+      <c r="G20" s="1">
+        <v>-0.27315899999999999</v>
+      </c>
+      <c r="H20" s="1">
+        <v>-0.124324</v>
+      </c>
+      <c r="I20" s="1">
+        <v>-8.9887999999999996E-2</v>
+      </c>
+      <c r="J20" s="1">
+        <v>3.6443000000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1">
+        <v>-0.21686</v>
+      </c>
+      <c r="C21" s="1">
+        <v>-9.5415E-2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-0.16644500000000001</v>
+      </c>
+      <c r="E21" s="1">
+        <v>-0.145679</v>
+      </c>
+      <c r="F21" s="1">
+        <v>-3.6651000000000003E-2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>-6.8640000000000007E-2</v>
+      </c>
+      <c r="H21" s="1">
+        <v>-7.8609999999999999E-2</v>
+      </c>
+      <c r="I21" s="1">
+        <v>-6.7552000000000001E-2</v>
+      </c>
+      <c r="J21" s="1">
+        <v>-3.7706999999999997E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1">
+        <v>-0.21201400000000001</v>
+      </c>
+      <c r="C22" s="1">
+        <v>-0.21595700000000001</v>
+      </c>
+      <c r="D22" s="1">
+        <v>-0.169817</v>
+      </c>
+      <c r="E22" s="1">
+        <v>-0.101364</v>
+      </c>
+      <c r="F22" s="1">
+        <v>-6.4235E-2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>-7.3653999999999997E-2</v>
+      </c>
+      <c r="H22" s="1">
+        <v>-4.8884999999999998E-2</v>
+      </c>
+      <c r="I22" s="1">
+        <v>-2.8972999999999999E-2</v>
+      </c>
+      <c r="J22" s="1">
+        <v>-1.1086E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>-0.20139199999999999</v>
+      </c>
+      <c r="C23" s="1">
+        <v>-0.165962</v>
+      </c>
+      <c r="D23" s="1">
+        <v>-0.34270800000000001</v>
+      </c>
+      <c r="E23" s="1">
+        <v>-0.29100999999999999</v>
+      </c>
+      <c r="F23" s="1">
+        <v>-0.24676699999999999</v>
+      </c>
+      <c r="G23" s="1">
+        <v>-0.186693</v>
+      </c>
+      <c r="H23" s="1">
+        <v>-6.2887999999999999E-2</v>
+      </c>
+      <c r="I23" s="1">
+        <v>-2.1257999999999999E-2</v>
+      </c>
+      <c r="J23" s="1">
+        <v>-8.3552000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1">
+        <v>-0.190053</v>
+      </c>
+      <c r="C24" s="1">
+        <v>-0.229796</v>
+      </c>
+      <c r="D24" s="1">
+        <v>-0.26002500000000001</v>
+      </c>
+      <c r="E24" s="1">
+        <v>-0.21589700000000001</v>
+      </c>
+      <c r="F24" s="1">
+        <v>-0.25876199999999999</v>
+      </c>
+      <c r="G24" s="1">
+        <v>-0.293182</v>
+      </c>
+      <c r="H24" s="1">
+        <v>-0.21441499999999999</v>
+      </c>
+      <c r="I24" s="1">
+        <v>-0.168132</v>
+      </c>
+      <c r="J24" s="1">
+        <v>-0.105381</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="1">
+        <v>-0.15451899999999999</v>
+      </c>
+      <c r="C25" s="1">
+        <v>-3.0099999999999998E-2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>-0.27815800000000002</v>
+      </c>
+      <c r="E25" s="1">
+        <v>-9.5163999999999999E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <v>8.4112099999999995E-2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>-9.1620999999999994E-2</v>
+      </c>
+      <c r="H25" s="1">
+        <v>-0.16184999999999999</v>
+      </c>
+      <c r="I25" s="1">
+        <v>-2.521E-2</v>
+      </c>
+      <c r="J25" s="1">
+        <v>4.4104400000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1">
+        <v>-0.15049299999999999</v>
+      </c>
+      <c r="C26" s="1">
+        <v>-0.14855599999999999</v>
+      </c>
+      <c r="D26" s="1">
+        <v>-8.3060999999999996E-2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>-5.8007999999999997E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <v>-8.4184999999999996E-2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>-6.3519000000000006E-2</v>
+      </c>
+      <c r="H26" s="1">
+        <v>-0.256963</v>
+      </c>
+      <c r="I26" s="1">
+        <v>-0.17791599999999999</v>
+      </c>
+      <c r="J26" s="1">
+        <v>-5.5227999999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1">
+        <v>-0.14997199999999999</v>
+      </c>
+      <c r="C27" s="1">
+        <v>-0.134687</v>
+      </c>
+      <c r="D27" s="1">
+        <v>-4.4761000000000002E-2</v>
+      </c>
+      <c r="E27" s="1">
+        <v>-4.3229999999999998E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <v>-5.5830999999999999E-2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>-1.6286999999999999E-2</v>
+      </c>
+      <c r="H27" s="1">
+        <v>-3.4580000000000001E-3</v>
+      </c>
+      <c r="I27" s="1">
+        <v>3.6769900000000001E-2</v>
+      </c>
+      <c r="J27" s="1">
+        <v>2.0771100000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="1">
+        <v>-0.14394799999999999</v>
+      </c>
+      <c r="C28" s="1">
+        <v>-0.15218899999999999</v>
+      </c>
+      <c r="D28" s="1">
+        <v>-0.33285199999999998</v>
+      </c>
+      <c r="E28" s="1">
+        <v>-0.33975899999999998</v>
+      </c>
+      <c r="F28" s="1">
+        <v>-0.19147500000000001</v>
+      </c>
+      <c r="G28" s="1">
+        <v>-0.12934000000000001</v>
+      </c>
+      <c r="H28" s="1">
+        <v>5.1001600000000001E-2</v>
+      </c>
+      <c r="I28" s="1">
+        <v>-0.137963</v>
+      </c>
+      <c r="J28" s="1">
+        <v>-0.153837</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1">
+        <v>-0.12940699999999999</v>
+      </c>
+      <c r="C29" s="1">
+        <v>-0.15668899999999999</v>
+      </c>
+      <c r="D29" s="1">
+        <v>-0.15265999999999999</v>
+      </c>
+      <c r="E29" s="1">
+        <v>-9.5921999999999993E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>-0.12432699999999999</v>
+      </c>
+      <c r="G29" s="1">
+        <v>-7.2939000000000004E-2</v>
+      </c>
+      <c r="H29" s="1">
+        <v>-0.122752</v>
+      </c>
+      <c r="I29" s="1">
+        <v>-0.12314600000000001</v>
+      </c>
+      <c r="J29" s="1">
+        <v>-3.5829E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1">
+        <v>-0.10915800000000001</v>
+      </c>
+      <c r="C30" s="1">
+        <v>-5.1334999999999999E-2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>-8.5813E-2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>-8.9649000000000006E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1.8983300000000002E-2</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1.5753E-2</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.17269139999999999</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.12932440000000001</v>
+      </c>
+      <c r="J30" s="1">
+        <v>7.2506299999999996E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="1">
+        <v>-0.107597</v>
+      </c>
+      <c r="C31" s="1">
+        <v>-0.107597</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.1292198</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.1292198</v>
+      </c>
+      <c r="F31" s="1">
+        <v>-8.2470000000000009E-3</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2.7670400000000001E-2</v>
+      </c>
+      <c r="H31" s="1">
+        <v>-0.22814799999999999</v>
+      </c>
+      <c r="I31" s="1">
+        <v>-1.186E-3</v>
+      </c>
+      <c r="J31" s="1">
+        <v>-5.6592999999999997E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="1">
+        <v>-7.6349E-2</v>
+      </c>
+      <c r="C32" s="1">
+        <v>-0.19423799999999999</v>
+      </c>
+      <c r="D32" s="1">
+        <v>-0.180787</v>
+      </c>
+      <c r="E32" s="1">
+        <v>-0.17224900000000001</v>
+      </c>
+      <c r="F32" s="1">
+        <v>-0.20153499999999999</v>
+      </c>
+      <c r="G32" s="1">
+        <v>-0.25563399999999997</v>
+      </c>
+      <c r="H32" s="1">
+        <v>-0.155862</v>
+      </c>
+      <c r="I32" s="1">
+        <v>-0.12002</v>
+      </c>
+      <c r="J32" s="1">
+        <v>-6.9575999999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="1">
+        <v>-6.7752000000000007E-2</v>
+      </c>
+      <c r="C33" s="1">
+        <v>-0.182586</v>
+      </c>
+      <c r="D33" s="1">
+        <v>-0.26034299999999999</v>
+      </c>
+      <c r="E33" s="1">
+        <v>-0.14524999999999999</v>
+      </c>
+      <c r="F33" s="1">
+        <v>-0.103195</v>
+      </c>
+      <c r="G33" s="1">
+        <v>-0.20413899999999999</v>
+      </c>
+      <c r="H33" s="1">
+        <v>-0.143424</v>
+      </c>
+      <c r="I33" s="1">
+        <v>-8.8931999999999997E-2</v>
+      </c>
+      <c r="J33" s="1">
+        <v>-7.2066000000000005E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="1">
+        <v>-5.4316000000000003E-2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>-2.5360000000000001E-3</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1.6097E-2</v>
+      </c>
+      <c r="E34" s="1">
+        <v>5.6696099999999999E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1.6097E-2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>4.0920199999999997E-2</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1.6770500000000001E-2</v>
+      </c>
+      <c r="I34" s="1">
+        <v>3.9130000000000002E-4</v>
+      </c>
+      <c r="J34" s="1">
+        <v>-5.3169999999999997E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="1">
+        <v>-2.7008000000000001E-2</v>
+      </c>
+      <c r="C35" s="1">
+        <v>6.7862699999999998E-2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>-0.15109500000000001</v>
+      </c>
+      <c r="E35" s="1">
+        <v>-0.21457300000000001</v>
+      </c>
+      <c r="F35" s="1">
+        <v>-0.112</v>
+      </c>
+      <c r="G35" s="1">
+        <v>-0.18382399999999999</v>
+      </c>
+      <c r="H35" s="1">
+        <v>-6.8284999999999998E-2</v>
+      </c>
+      <c r="I35" s="1">
+        <v>-2.0042999999999998E-2</v>
+      </c>
+      <c r="J35" s="1">
+        <v>8.7370900000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="1">
+        <v>-8.4840000000000002E-3</v>
+      </c>
+      <c r="C36" s="1">
+        <v>-0.19422400000000001</v>
+      </c>
+      <c r="D36" s="1">
+        <v>-0.10993</v>
+      </c>
+      <c r="E36" s="1">
+        <v>-0.23738000000000001</v>
+      </c>
+      <c r="F36" s="1">
+        <v>-0.31093599999999999</v>
+      </c>
+      <c r="G36" s="1">
+        <v>-0.39494000000000001</v>
+      </c>
+      <c r="H36" s="1">
+        <v>-0.278173</v>
+      </c>
+      <c r="I36" s="1">
+        <v>-0.14940999999999999</v>
+      </c>
+      <c r="J36" s="1">
+        <v>-4.4430999999999998E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2.4580000000000001E-3</v>
+      </c>
+      <c r="C37" s="1">
+        <v>-3.9639000000000001E-2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>-4.8847000000000002E-2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>-6.7099000000000006E-2</v>
+      </c>
+      <c r="F37" s="1">
+        <v>-2.0546999999999999E-2</v>
+      </c>
+      <c r="G37" s="1">
+        <v>-5.2040000000000003E-2</v>
+      </c>
+      <c r="H37" s="1">
+        <v>-0.106282</v>
+      </c>
+      <c r="I37" s="1">
+        <v>-0.123672</v>
+      </c>
+      <c r="J37" s="1">
+        <v>-2.7167E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="1">
+        <v>6.5510000000000004E-3</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4.3310700000000001E-2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>-0.12873599999999999</v>
+      </c>
+      <c r="E38" s="1">
+        <v>-0.102321</v>
+      </c>
+      <c r="F38" s="1">
+        <v>-1.7285999999999999E-2</v>
+      </c>
+      <c r="G38" s="1">
+        <v>-5.6744999999999997E-2</v>
+      </c>
+      <c r="H38" s="1">
+        <v>-6.8643999999999997E-2</v>
+      </c>
+      <c r="I38" s="1">
+        <v>-6.1107000000000002E-2</v>
+      </c>
+      <c r="J38" s="1">
+        <v>-6.1416999999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1">
+        <v>8.4825999999999999E-3</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.1468382</v>
+      </c>
+      <c r="D39" s="1">
+        <v>-5.3096999999999998E-2</v>
+      </c>
+      <c r="E39" s="1">
+        <v>8.9612999999999998E-2</v>
+      </c>
+      <c r="F39" s="1">
+        <v>3.3816400000000003E-2</v>
+      </c>
+      <c r="G39" s="1">
+        <v>6.1507899999999997E-2</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0.13107820000000001</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0.1875694</v>
+      </c>
+      <c r="J39" s="1">
+        <v>0.1227702</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2.52959E-2</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.46679949999999998</v>
+      </c>
+      <c r="D40" s="1">
+        <v>8.5503700000000002E-2</v>
+      </c>
+      <c r="E40" s="1">
+        <v>6.4834900000000001E-2</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.52344829999999998</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.375467</v>
+      </c>
+      <c r="H40" s="1">
+        <v>7.0251900000000006E-2</v>
+      </c>
+      <c r="I40" s="1">
+        <v>6.9215899999999997E-2</v>
+      </c>
+      <c r="J40" s="1">
+        <v>-2.2134000000000001E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="1">
+        <v>6.82141E-2</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.29746840000000002</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.19186049999999999</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.11413040000000001</v>
+      </c>
+      <c r="F41" s="1">
+        <v>-0.101951</v>
+      </c>
+      <c r="G41" s="1">
+        <v>-0.15983600000000001</v>
+      </c>
+      <c r="H41" s="1">
+        <v>-0.16264400000000001</v>
+      </c>
+      <c r="I41" s="1">
+        <v>-0.189723</v>
+      </c>
+      <c r="J41" s="1">
+        <v>-0.12867100000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="1">
+        <v>7.9227099999999995E-2</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0.1708595</v>
+      </c>
+      <c r="D42" s="1">
+        <v>-7.9901E-2</v>
+      </c>
+      <c r="E42" s="1">
+        <v>-8.4426000000000001E-2</v>
+      </c>
+      <c r="F42" s="1">
+        <v>-2.3601E-2</v>
+      </c>
+      <c r="G42" s="1">
+        <v>-3.7068999999999998E-2</v>
+      </c>
+      <c r="H42" s="1">
+        <v>-0.23177400000000001</v>
+      </c>
+      <c r="I42" s="1">
+        <v>-0.28351500000000002</v>
+      </c>
+      <c r="J42" s="1">
+        <v>-0.26657900000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.1207023</v>
+      </c>
+      <c r="C43" s="1">
+        <v>-8.4279999999999994E-2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>-9.3491000000000005E-2</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1.6589300000000001E-2</v>
+      </c>
+      <c r="F43" s="1">
+        <v>-2.2336000000000002E-2</v>
+      </c>
+      <c r="G43" s="1">
+        <v>4.6448099999999999E-2</v>
+      </c>
+      <c r="H43" s="1">
+        <v>-6.4850000000000003E-3</v>
+      </c>
+      <c r="I43" s="1">
+        <v>-1.8578000000000001E-2</v>
+      </c>
+      <c r="J43" s="1">
+        <v>-5.5180000000000003E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.18148600000000001</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0.17861479999999999</v>
+      </c>
+      <c r="D44" s="1">
+        <v>-2.6103999999999999E-2</v>
+      </c>
+      <c r="E44" s="1">
+        <v>4.1331199999999998E-2</v>
+      </c>
+      <c r="F44" s="1">
+        <v>-8.8345999999999994E-2</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1.4114E-2</v>
+      </c>
+      <c r="H44" s="1">
+        <v>-3.0829999999999998E-3</v>
+      </c>
+      <c r="I44" s="1">
+        <v>8.7443900000000005E-2</v>
+      </c>
+      <c r="J44" s="1">
+        <v>-8.1799999999999998E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.23304349999999999</v>
+      </c>
+      <c r="C45" s="1">
+        <v>7.0569999999999997E-4</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.1856187</v>
+      </c>
+      <c r="E45" s="1">
+        <v>-0.12198100000000001</v>
+      </c>
+      <c r="F45" s="1">
+        <v>-0.197964</v>
+      </c>
+      <c r="G45" s="1">
+        <v>-0.226405</v>
+      </c>
+      <c r="H45" s="1">
+        <v>-0.24494099999999999</v>
+      </c>
+      <c r="I45" s="1">
+        <v>-0.187393</v>
+      </c>
+      <c r="J45" s="1">
+        <v>-0.17027500000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.26216410000000001</v>
+      </c>
+      <c r="C46" s="1">
+        <v>-0.113717</v>
+      </c>
+      <c r="D46" s="1">
+        <v>-0.37862000000000001</v>
+      </c>
+      <c r="E46" s="1">
+        <v>-0.36638700000000002</v>
+      </c>
+      <c r="F46" s="1">
+        <v>-0.24631400000000001</v>
+      </c>
+      <c r="G46" s="1">
+        <v>-0.27973500000000001</v>
+      </c>
+      <c r="H46" s="1">
+        <v>-0.27673700000000001</v>
+      </c>
+      <c r="I46" s="1">
+        <v>-0.21922700000000001</v>
+      </c>
+      <c r="J46" s="1">
+        <v>-0.12354999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.28473409999999999</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.53483610000000004</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.15884480000000001</v>
+      </c>
+      <c r="E47" s="1">
+        <v>-4.2199E-2</v>
+      </c>
+      <c r="F47" s="1">
+        <v>2.18281E-2</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.14176830000000001</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0.26165080000000002</v>
+      </c>
+      <c r="I47" s="1">
+        <v>6.7965800000000007E-2</v>
+      </c>
+      <c r="J47" s="1">
+        <v>0.1429298</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.29622530000000002</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.35171649999999999</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.26650299999999999</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.1779406</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0.1766683</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.1203931</v>
+      </c>
+      <c r="H48" s="1">
+        <v>3.0427200000000001E-2</v>
+      </c>
+      <c r="I48" s="1">
+        <v>-7.6705999999999996E-2</v>
+      </c>
+      <c r="J48" s="1">
+        <v>-7.2249999999999995E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.3049423</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.30688009999999999</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.36994120000000003</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0.35773050000000001</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0.28005819999999998</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0.26817160000000001</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0.2503552</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0.1449841</v>
+      </c>
+      <c r="J49" s="1">
+        <v>3.9501300000000003E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.37940289999999999</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.41271170000000001</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.41405340000000002</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0.31622109999999998</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0.36105290000000001</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0.24129600000000001</v>
+      </c>
+      <c r="H50" s="1">
+        <v>0.1152267</v>
+      </c>
+      <c r="I50" s="1">
+        <v>7.1497699999999997E-2</v>
+      </c>
+      <c r="J50" s="1">
+        <v>-2.1506999999999998E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.45125789999999999</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0.50081299999999995</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.19404920000000001</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.155194</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0.53067989999999998</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0.34156979999999998</v>
+      </c>
+      <c r="H51" s="1">
+        <v>-0.55389100000000002</v>
+      </c>
+      <c r="I51" s="1">
+        <v>-0.26629599999999998</v>
+      </c>
+      <c r="J51" s="1">
+        <v>-0.29271999999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.49655169999999998</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0.49655169999999998</v>
+      </c>
+      <c r="D52" s="1">
+        <v>-2.7569999999999999E-3</v>
+      </c>
+      <c r="E52" s="1">
+        <v>-0.336391</v>
+      </c>
+      <c r="F52" s="1">
+        <v>-0.37822299999999998</v>
+      </c>
+      <c r="G52" s="1">
+        <v>-0.16602600000000001</v>
+      </c>
+      <c r="H52" s="1">
+        <v>-0.146341</v>
+      </c>
+      <c r="I52" s="1">
+        <v>-0.199853</v>
+      </c>
+      <c r="J52" s="1">
+        <v>-0.15234400000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0.56954890000000002</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.38153540000000002</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.3407193</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0.27695370000000002</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0.2755881</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0.2007478</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0.2163146</v>
+      </c>
+      <c r="I53" s="1">
+        <v>7.7697500000000003E-2</v>
+      </c>
+      <c r="J53" s="1">
+        <v>0.1441491</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.59590319999999997</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0.1411451</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.66407769999999999</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0.48013820000000001</v>
+      </c>
+      <c r="F54" s="1">
+        <v>-0.174374</v>
+      </c>
+      <c r="G54" s="1">
+        <v>-0.52730299999999997</v>
+      </c>
+      <c r="H54" s="1">
+        <v>-0.10073500000000001</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0.13210040000000001</v>
+      </c>
+      <c r="J54" s="1">
+        <v>7.3934799999999995E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.851468</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0.851468</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0.46648430000000002</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0.46648430000000002</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0.2978208</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0.24796270000000001</v>
+      </c>
+      <c r="H55" s="1">
+        <v>-2.0109999999999999E-2</v>
+      </c>
+      <c r="I55" s="1">
+        <v>0.2112994</v>
+      </c>
+      <c r="J55" s="1">
+        <v>3.4749000000000002E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J55" xr:uid="{B7E36668-8DF2-4137-A061-9502B5B6A8F9}">
+    <sortState ref="A2:J55">
+      <sortCondition ref="B1:B55"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{EC5F9957-9097-4B86-9D86-09868EB4E77C}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B2:J2</xm:f>
+              <xm:sqref>K2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B3:J3</xm:f>
+              <xm:sqref>K3</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B4:J4</xm:f>
+              <xm:sqref>K4</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B5:J5</xm:f>
+              <xm:sqref>K5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B6:J6</xm:f>
+              <xm:sqref>K6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B7:J7</xm:f>
+              <xm:sqref>K7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B8:J8</xm:f>
+              <xm:sqref>K8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B9:J9</xm:f>
+              <xm:sqref>K9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B10:J10</xm:f>
+              <xm:sqref>K10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B11:J11</xm:f>
+              <xm:sqref>K11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B12:J12</xm:f>
+              <xm:sqref>K12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B13:J13</xm:f>
+              <xm:sqref>K13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B14:J14</xm:f>
+              <xm:sqref>K14</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B15:J15</xm:f>
+              <xm:sqref>K15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B16:J16</xm:f>
+              <xm:sqref>K16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B17:J17</xm:f>
+              <xm:sqref>K17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B18:J18</xm:f>
+              <xm:sqref>K18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B19:J19</xm:f>
+              <xm:sqref>K19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B20:J20</xm:f>
+              <xm:sqref>K20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B21:J21</xm:f>
+              <xm:sqref>K21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B22:J22</xm:f>
+              <xm:sqref>K22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B23:J23</xm:f>
+              <xm:sqref>K23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B24:J24</xm:f>
+              <xm:sqref>K24</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B25:J25</xm:f>
+              <xm:sqref>K25</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B26:J26</xm:f>
+              <xm:sqref>K26</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B27:J27</xm:f>
+              <xm:sqref>K27</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B28:J28</xm:f>
+              <xm:sqref>K28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B29:J29</xm:f>
+              <xm:sqref>K29</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B30:J30</xm:f>
+              <xm:sqref>K30</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B31:J31</xm:f>
+              <xm:sqref>K31</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B32:J32</xm:f>
+              <xm:sqref>K32</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B33:J33</xm:f>
+              <xm:sqref>K33</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B34:J34</xm:f>
+              <xm:sqref>K34</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B35:J35</xm:f>
+              <xm:sqref>K35</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B36:J36</xm:f>
+              <xm:sqref>K36</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B37:J37</xm:f>
+              <xm:sqref>K37</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B38:J38</xm:f>
+              <xm:sqref>K38</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B39:J39</xm:f>
+              <xm:sqref>K39</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B40:J40</xm:f>
+              <xm:sqref>K40</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B41:J41</xm:f>
+              <xm:sqref>K41</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B42:J42</xm:f>
+              <xm:sqref>K42</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B43:J43</xm:f>
+              <xm:sqref>K43</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B44:J44</xm:f>
+              <xm:sqref>K44</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B45:J45</xm:f>
+              <xm:sqref>K45</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B46:J46</xm:f>
+              <xm:sqref>K46</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B47:J47</xm:f>
+              <xm:sqref>K47</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B48:J48</xm:f>
+              <xm:sqref>K48</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B49:J49</xm:f>
+              <xm:sqref>K49</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B50:J50</xm:f>
+              <xm:sqref>K50</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B51:J51</xm:f>
+              <xm:sqref>K51</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B52:J52</xm:f>
+              <xm:sqref>K52</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B53:J53</xm:f>
+              <xm:sqref>K53</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B54:J54</xm:f>
+              <xm:sqref>K54</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Variation-with-TrendLines'!B55:J55</xm:f>
+              <xm:sqref>K55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>